<commit_message>
added routines for CMIP3 GWLs
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP5_all_models.xlsx
+++ b/data/gwl_lists/GWLs_CMIP5_all_models.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10333F2-83B4-7649-B888-9D80D97E2658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A614E-8145-2345-A84E-8477B4D19278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" xr2:uid="{F14C9CA9-83D9-2B46-A323-DF5833BB358B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Model</t>
   </si>
@@ -264,14 +264,24 @@
   </si>
   <si>
     <t>AUT GCM CCS 1991-2020</t>
+  </si>
+  <si>
+    <t>GFDL-CM3_rcp85_r1i1p1_200601-210012</t>
+  </si>
+  <si>
+    <t>2045-2064</t>
+  </si>
+  <si>
+    <t>2061-2080</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -323,10 +333,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD54D6C1-6F42-F64D-905A-EC4D8AA38A62}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,31 +666,31 @@
     <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1256,192 +1267,236 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B23">
-        <v>2011</v>
+        <v>2023</v>
       </c>
       <c r="C23">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="D23">
-        <v>2048</v>
+        <v>2055</v>
       </c>
       <c r="E23">
-        <v>2066</v>
+        <v>2071</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="J23" s="2">
-        <v>0.27716342078308198</v>
+        <v>1.2547776910347199</v>
       </c>
       <c r="K23" s="2">
-        <v>0.97698444790303796</v>
+        <v>1.8814544179047701</v>
       </c>
       <c r="L23" s="2">
-        <v>2.1671324835882499</v>
+        <v>3.3167032989732199</v>
       </c>
       <c r="M23" s="2">
-        <v>3.4109224743312501</v>
+        <v>4.9136741564842401</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24">
-        <v>2034</v>
+        <v>2011</v>
       </c>
       <c r="C24">
+        <v>2027</v>
+      </c>
+      <c r="D24">
         <v>2048</v>
       </c>
-      <c r="D24">
-        <v>2070</v>
+      <c r="E24">
+        <v>2066</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" t="s">
         <v>62</v>
       </c>
-      <c r="H24" t="s">
-        <v>40</v>
+      <c r="I24" t="s">
+        <v>63</v>
       </c>
       <c r="J24" s="2">
-        <v>0.69072337680391005</v>
+        <v>0.27716342078308198</v>
       </c>
       <c r="K24" s="2">
-        <v>1.39141197204587</v>
+        <v>0.97698444790303796</v>
       </c>
       <c r="L24" s="2">
-        <v>2.5225286695692</v>
-      </c>
-      <c r="M24" s="2"/>
+        <v>2.1671324835882499</v>
+      </c>
+      <c r="M24" s="2">
+        <v>3.4109224743312501</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="C25">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D25">
-        <v>2074</v>
+        <v>2070</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J25" s="2">
-        <v>0.78084819934989003</v>
+        <v>0.69072337680391005</v>
       </c>
       <c r="K25" s="2">
-        <v>1.1650189858895901</v>
+        <v>1.39141197204587</v>
       </c>
       <c r="L25" s="2">
-        <v>2.51032525521738</v>
+        <v>2.5225286695692</v>
       </c>
       <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26">
-        <v>2011</v>
+        <v>2033</v>
       </c>
       <c r="C26">
-        <v>2029</v>
+        <v>2050</v>
       </c>
       <c r="D26">
-        <v>2060</v>
-      </c>
-      <c r="E26">
-        <v>2086</v>
+        <v>2074</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H26" t="s">
-        <v>69</v>
-      </c>
-      <c r="I26" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="J26" s="2">
-        <v>0.19708605850399499</v>
+        <v>0.78084819934989003</v>
       </c>
       <c r="K26" s="2">
-        <v>0.85248630903591305</v>
+        <v>1.1650189858895901</v>
       </c>
       <c r="L26" s="2">
-        <v>2.72245074781776</v>
-      </c>
-      <c r="M26" s="2">
-        <v>3.5750805834353399</v>
-      </c>
+        <v>2.51032525521738</v>
+      </c>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="C27">
-        <v>2037</v>
+        <v>2029</v>
       </c>
       <c r="D27">
         <v>2060</v>
       </c>
       <c r="E27">
-        <v>2084</v>
+        <v>2086</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H27" t="s">
         <v>69</v>
       </c>
       <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.19708605850399499</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.85248630903591305</v>
+      </c>
+      <c r="L27" s="2">
+        <v>2.72245074781776</v>
+      </c>
+      <c r="M27" s="2">
+        <v>3.5750805834353399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28">
+        <v>2020</v>
+      </c>
+      <c r="C28">
+        <v>2037</v>
+      </c>
+      <c r="D28">
+        <v>2060</v>
+      </c>
+      <c r="E28">
+        <v>2084</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J28" s="2">
         <v>0.25636699817790398</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K28" s="2">
         <v>1.4150692127368201</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L28" s="2">
         <v>2.2598840219002199</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M28" s="2">
         <v>3.8378899609600099</v>
       </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>